<commit_message>
RM-81 Part II: Adds a (temporary) menu and Users only see there own Contracts (with contract_name = name_in_negometrix)
</commit_message>
<xml_diff>
--- a/rm/test/resources/Overzicht Tech Cluster Backend 2-12.xlsx
+++ b/rm/test/resources/Overzicht Tech Cluster Backend 2-12.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t xml:space="preserve">Database nr.</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t xml:space="preserve">44337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eelco Aartsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eelco@aesset.nl</t>
   </si>
 </sst>
 </file>
@@ -169,7 +175,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -194,6 +200,13 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -248,7 +261,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="1" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,6 +286,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,8 +309,8 @@
   </sheetPr>
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -302,7 +319,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="63.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="6" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="38.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="8" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="12.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.5"/>
@@ -620,7 +639,77 @@
         <v>40969.4583333333</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>44256.4583333333</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="5" t="n">
+        <v>2656</v>
+      </c>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="4" t="n">
+        <v>41334.4583333333</v>
+      </c>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG5" s="4" t="n">
+        <v>40969.4583333333</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -799,6 +888,9 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" display="eelco@aesset.nl"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>